<commit_message>
fix and rename files
</commit_message>
<xml_diff>
--- a/data/fix_values.xlsx
+++ b/data/fix_values.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anderson/google_drive/ITpS/projetos_itps/resp_pathogens/analyses/20220215_relatorio2/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Anderson/Library/CloudStorage/GoogleDrive-anderson.brito@itps.org.br/Outros computadores/My Mac mini/google_drive/ITpS/projetos_itps/resp_pathogens/analyses/itps_respat_test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5F0495-68D2-C743-951D-304BF51796CB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1B02CD-41AD-2540-8CB6-B3292767414D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28600" yWindow="18060" windowWidth="11360" windowHeight="17480" xr2:uid="{85AFBA56-08BE-0441-AF99-E499752AA002}"/>
+    <workbookView xWindow="-22440" yWindow="500" windowWidth="11360" windowHeight="17480" xr2:uid="{85AFBA56-08BE-0441-AF99-E499752AA002}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="615">
   <si>
     <t>lab_id</t>
   </si>
@@ -135,9 +135,6 @@
     <t>Planaltina</t>
   </si>
   <si>
-    <t>DASA_2</t>
-  </si>
-  <si>
     <t>SAOPAULO</t>
   </si>
   <si>
@@ -1860,10 +1857,19 @@
     <t>NAO DETECTADO</t>
   </si>
   <si>
-    <t>DB Molecular_2</t>
-  </si>
-  <si>
     <t>Não detectado</t>
+  </si>
+  <si>
+    <t>DASA</t>
+  </si>
+  <si>
+    <t>Detectado (Presença do RNA de Coronavírus SARS-CoV</t>
+  </si>
+  <si>
+    <t>Inconclusivo</t>
+  </si>
+  <si>
+    <t>Não detectado (Ausência do RNA de Coronavírus SARS</t>
   </si>
 </sst>
 </file>
@@ -2223,10 +2229,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1713BFE-4562-D640-92D5-BBA09EA5AB16}">
-  <dimension ref="A1:D387"/>
+  <dimension ref="A1:D390"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2701,13 +2707,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B34" t="s">
         <v>12</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>612</v>
       </c>
       <c r="D34" t="s">
         <v>4</v>
@@ -2715,13 +2721,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B35" t="s">
         <v>12</v>
       </c>
       <c r="C35" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="D35" t="s">
         <v>5</v>
@@ -2729,16 +2735,16 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>611</v>
+        <v>23</v>
       </c>
       <c r="B36" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>4</v>
+      <c r="C36" t="s">
+        <v>614</v>
+      </c>
+      <c r="D36" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -2748,53 +2754,53 @@
       <c r="B37" t="s">
         <v>12</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>612</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>5</v>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>611</v>
       </c>
       <c r="B38" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>15</v>
+        <v>609</v>
       </c>
       <c r="D38" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39" t="s">
-        <v>17</v>
-      </c>
-      <c r="D39" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" t="s">
-        <v>19</v>
-      </c>
-      <c r="D40" t="s">
-        <v>20</v>
+        <v>12</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -2805,10 +2811,10 @@
         <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D41" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -2819,10 +2825,10 @@
         <v>14</v>
       </c>
       <c r="C42" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D42" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -2833,10 +2839,10 @@
         <v>14</v>
       </c>
       <c r="C43" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="D43" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -2847,10 +2853,10 @@
         <v>14</v>
       </c>
       <c r="C44" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="D44" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -2861,10 +2867,10 @@
         <v>14</v>
       </c>
       <c r="C45" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D45" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -2875,10 +2881,10 @@
         <v>14</v>
       </c>
       <c r="C46" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D46" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -2889,10 +2895,10 @@
         <v>14</v>
       </c>
       <c r="C47" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D47" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -2903,10 +2909,10 @@
         <v>14</v>
       </c>
       <c r="C48" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D48" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -2917,10 +2923,10 @@
         <v>14</v>
       </c>
       <c r="C49" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D49" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -2931,10 +2937,10 @@
         <v>14</v>
       </c>
       <c r="C50" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D50" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -2945,10 +2951,10 @@
         <v>14</v>
       </c>
       <c r="C51" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D51" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -2959,10 +2965,10 @@
         <v>14</v>
       </c>
       <c r="C52" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D52" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -2973,10 +2979,10 @@
         <v>14</v>
       </c>
       <c r="C53" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D53" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -2987,10 +2993,10 @@
         <v>14</v>
       </c>
       <c r="C54" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D54" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -3001,10 +3007,10 @@
         <v>14</v>
       </c>
       <c r="C55" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D55" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -3015,10 +3021,10 @@
         <v>14</v>
       </c>
       <c r="C56" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D56" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -3029,10 +3035,10 @@
         <v>14</v>
       </c>
       <c r="C57" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D57" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -3043,10 +3049,10 @@
         <v>14</v>
       </c>
       <c r="C58" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D58" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -3057,10 +3063,10 @@
         <v>14</v>
       </c>
       <c r="C59" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D59" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -3071,10 +3077,10 @@
         <v>14</v>
       </c>
       <c r="C60" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D60" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -3085,10 +3091,10 @@
         <v>14</v>
       </c>
       <c r="C61" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D61" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -3099,10 +3105,10 @@
         <v>14</v>
       </c>
       <c r="C62" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D62" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -3113,10 +3119,10 @@
         <v>14</v>
       </c>
       <c r="C63" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D63" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -3127,10 +3133,10 @@
         <v>14</v>
       </c>
       <c r="C64" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D64" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -3141,10 +3147,10 @@
         <v>14</v>
       </c>
       <c r="C65" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D65" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -3155,10 +3161,10 @@
         <v>14</v>
       </c>
       <c r="C66" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D66" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -3169,10 +3175,10 @@
         <v>14</v>
       </c>
       <c r="C67" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D67" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -3183,10 +3189,10 @@
         <v>14</v>
       </c>
       <c r="C68" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D68" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -3197,10 +3203,10 @@
         <v>14</v>
       </c>
       <c r="C69" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D69" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -3211,10 +3217,10 @@
         <v>14</v>
       </c>
       <c r="C70" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D70" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -3225,10 +3231,10 @@
         <v>14</v>
       </c>
       <c r="C71" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D71" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -3239,10 +3245,10 @@
         <v>14</v>
       </c>
       <c r="C72" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D72" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -3253,10 +3259,10 @@
         <v>14</v>
       </c>
       <c r="C73" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D73" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -3267,10 +3273,10 @@
         <v>14</v>
       </c>
       <c r="C74" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D74" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -3281,10 +3287,10 @@
         <v>14</v>
       </c>
       <c r="C75" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D75" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -3295,10 +3301,10 @@
         <v>14</v>
       </c>
       <c r="C76" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D76" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -3309,10 +3315,10 @@
         <v>14</v>
       </c>
       <c r="C77" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D77" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -3323,10 +3329,10 @@
         <v>14</v>
       </c>
       <c r="C78" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D78" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -3337,10 +3343,10 @@
         <v>14</v>
       </c>
       <c r="C79" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D79" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -3351,10 +3357,10 @@
         <v>14</v>
       </c>
       <c r="C80" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D80" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -3365,10 +3371,10 @@
         <v>14</v>
       </c>
       <c r="C81" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D81" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -3379,10 +3385,10 @@
         <v>14</v>
       </c>
       <c r="C82" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D82" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -3393,10 +3399,10 @@
         <v>14</v>
       </c>
       <c r="C83" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D83" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -3407,10 +3413,10 @@
         <v>14</v>
       </c>
       <c r="C84" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D84" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -3421,10 +3427,10 @@
         <v>14</v>
       </c>
       <c r="C85" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D85" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -3435,10 +3441,10 @@
         <v>14</v>
       </c>
       <c r="C86" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D86" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -3449,10 +3455,10 @@
         <v>14</v>
       </c>
       <c r="C87" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D87" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -3463,10 +3469,10 @@
         <v>14</v>
       </c>
       <c r="C88" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D88" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -3477,10 +3483,10 @@
         <v>14</v>
       </c>
       <c r="C89" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="D89" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -3491,10 +3497,10 @@
         <v>14</v>
       </c>
       <c r="C90" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D90" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -3505,10 +3511,10 @@
         <v>14</v>
       </c>
       <c r="C91" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D91" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -3519,10 +3525,10 @@
         <v>14</v>
       </c>
       <c r="C92" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D92" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -3533,10 +3539,10 @@
         <v>14</v>
       </c>
       <c r="C93" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D93" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -3547,10 +3553,10 @@
         <v>14</v>
       </c>
       <c r="C94" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="D94" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -3561,10 +3567,10 @@
         <v>14</v>
       </c>
       <c r="C95" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D95" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -3575,10 +3581,10 @@
         <v>14</v>
       </c>
       <c r="C96" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D96" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -3589,10 +3595,10 @@
         <v>14</v>
       </c>
       <c r="C97" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D97" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -3603,10 +3609,10 @@
         <v>14</v>
       </c>
       <c r="C98" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D98" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
@@ -3617,10 +3623,10 @@
         <v>14</v>
       </c>
       <c r="C99" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D99" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -3631,10 +3637,10 @@
         <v>14</v>
       </c>
       <c r="C100" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D100" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -3645,10 +3651,10 @@
         <v>14</v>
       </c>
       <c r="C101" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D101" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -3659,10 +3665,10 @@
         <v>14</v>
       </c>
       <c r="C102" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="D102" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -3673,10 +3679,10 @@
         <v>14</v>
       </c>
       <c r="C103" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D103" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -3687,10 +3693,10 @@
         <v>14</v>
       </c>
       <c r="C104" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="D104" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
@@ -3701,10 +3707,10 @@
         <v>14</v>
       </c>
       <c r="C105" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="D105" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -3715,10 +3721,10 @@
         <v>14</v>
       </c>
       <c r="C106" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D106" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
@@ -3729,10 +3735,10 @@
         <v>14</v>
       </c>
       <c r="C107" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="D107" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
@@ -3743,10 +3749,10 @@
         <v>14</v>
       </c>
       <c r="C108" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="D108" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
@@ -3757,10 +3763,10 @@
         <v>14</v>
       </c>
       <c r="C109" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="D109" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
@@ -3771,10 +3777,10 @@
         <v>14</v>
       </c>
       <c r="C110" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D110" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
@@ -3785,10 +3791,10 @@
         <v>14</v>
       </c>
       <c r="C111" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D111" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
@@ -3799,10 +3805,10 @@
         <v>14</v>
       </c>
       <c r="C112" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D112" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -3813,10 +3819,10 @@
         <v>14</v>
       </c>
       <c r="C113" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D113" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
@@ -3827,10 +3833,10 @@
         <v>14</v>
       </c>
       <c r="C114" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D114" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
@@ -3841,10 +3847,10 @@
         <v>14</v>
       </c>
       <c r="C115" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="D115" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
@@ -3855,10 +3861,10 @@
         <v>14</v>
       </c>
       <c r="C116" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D116" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
@@ -3869,10 +3875,10 @@
         <v>14</v>
       </c>
       <c r="C117" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D117" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
@@ -3883,10 +3889,10 @@
         <v>14</v>
       </c>
       <c r="C118" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="D118" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
@@ -3897,10 +3903,10 @@
         <v>14</v>
       </c>
       <c r="C119" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="D119" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
@@ -3911,10 +3917,10 @@
         <v>14</v>
       </c>
       <c r="C120" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="D120" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
@@ -3925,10 +3931,10 @@
         <v>14</v>
       </c>
       <c r="C121" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="D121" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
@@ -3939,10 +3945,10 @@
         <v>14</v>
       </c>
       <c r="C122" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="D122" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
@@ -3953,10 +3959,10 @@
         <v>14</v>
       </c>
       <c r="C123" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="D123" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
@@ -3967,10 +3973,10 @@
         <v>14</v>
       </c>
       <c r="C124" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="D124" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
@@ -3981,10 +3987,10 @@
         <v>14</v>
       </c>
       <c r="C125" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="D125" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
@@ -3995,10 +4001,10 @@
         <v>14</v>
       </c>
       <c r="C126" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="D126" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
@@ -4009,10 +4015,10 @@
         <v>14</v>
       </c>
       <c r="C127" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="D127" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
@@ -4023,10 +4029,10 @@
         <v>14</v>
       </c>
       <c r="C128" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D128" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
@@ -4037,10 +4043,10 @@
         <v>14</v>
       </c>
       <c r="C129" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="D129" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
@@ -4051,10 +4057,10 @@
         <v>14</v>
       </c>
       <c r="C130" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="D130" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
@@ -4065,10 +4071,10 @@
         <v>14</v>
       </c>
       <c r="C131" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="D131" t="s">
-        <v>42</v>
+        <v>207</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
@@ -4079,10 +4085,10 @@
         <v>14</v>
       </c>
       <c r="C132" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D132" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
@@ -4093,10 +4099,10 @@
         <v>14</v>
       </c>
       <c r="C133" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="D133" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
@@ -4107,10 +4113,10 @@
         <v>14</v>
       </c>
       <c r="C134" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="D134" t="s">
-        <v>219</v>
+        <v>41</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
@@ -4121,10 +4127,10 @@
         <v>14</v>
       </c>
       <c r="C135" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="D135" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
@@ -4135,10 +4141,10 @@
         <v>14</v>
       </c>
       <c r="C136" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D136" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
@@ -4149,10 +4155,10 @@
         <v>14</v>
       </c>
       <c r="C137" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="D137" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
@@ -4163,10 +4169,10 @@
         <v>14</v>
       </c>
       <c r="C138" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="D138" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
@@ -4177,10 +4183,10 @@
         <v>14</v>
       </c>
       <c r="C139" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D139" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
@@ -4191,10 +4197,10 @@
         <v>14</v>
       </c>
       <c r="C140" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D140" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
@@ -4205,10 +4211,10 @@
         <v>14</v>
       </c>
       <c r="C141" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D141" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
@@ -4219,10 +4225,10 @@
         <v>14</v>
       </c>
       <c r="C142" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="D142" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
@@ -4233,10 +4239,10 @@
         <v>14</v>
       </c>
       <c r="C143" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="D143" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
@@ -4247,10 +4253,10 @@
         <v>14</v>
       </c>
       <c r="C144" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="D144" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
@@ -4261,10 +4267,10 @@
         <v>14</v>
       </c>
       <c r="C145" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="D145" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
@@ -4275,10 +4281,10 @@
         <v>14</v>
       </c>
       <c r="C146" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D146" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
@@ -4289,10 +4295,10 @@
         <v>14</v>
       </c>
       <c r="C147" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="D147" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
@@ -4303,10 +4309,10 @@
         <v>14</v>
       </c>
       <c r="C148" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="D148" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
@@ -4317,10 +4323,10 @@
         <v>14</v>
       </c>
       <c r="C149" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="D149" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
@@ -4331,10 +4337,10 @@
         <v>14</v>
       </c>
       <c r="C150" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="D150" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
@@ -4345,10 +4351,10 @@
         <v>14</v>
       </c>
       <c r="C151" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="D151" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
@@ -4359,10 +4365,10 @@
         <v>14</v>
       </c>
       <c r="C152" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="D152" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
@@ -4373,10 +4379,10 @@
         <v>14</v>
       </c>
       <c r="C153" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="D153" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
@@ -4387,10 +4393,10 @@
         <v>14</v>
       </c>
       <c r="C154" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="D154" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
@@ -4401,10 +4407,10 @@
         <v>14</v>
       </c>
       <c r="C155" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="D155" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
@@ -4415,10 +4421,10 @@
         <v>14</v>
       </c>
       <c r="C156" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="D156" t="s">
-        <v>66</v>
+        <v>256</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
@@ -4429,10 +4435,10 @@
         <v>14</v>
       </c>
       <c r="C157" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="D157" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
@@ -4443,10 +4449,10 @@
         <v>14</v>
       </c>
       <c r="C158" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D158" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
@@ -4457,10 +4463,10 @@
         <v>14</v>
       </c>
       <c r="C159" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="D159" t="s">
-        <v>264</v>
+        <v>65</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
@@ -4471,10 +4477,10 @@
         <v>14</v>
       </c>
       <c r="C160" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D160" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
@@ -4485,10 +4491,10 @@
         <v>14</v>
       </c>
       <c r="C161" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D161" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
@@ -4499,10 +4505,10 @@
         <v>14</v>
       </c>
       <c r="C162" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D162" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
@@ -4513,10 +4519,10 @@
         <v>14</v>
       </c>
       <c r="C163" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="D163" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
@@ -4527,10 +4533,10 @@
         <v>14</v>
       </c>
       <c r="C164" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="D164" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
@@ -4541,10 +4547,10 @@
         <v>14</v>
       </c>
       <c r="C165" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="D165" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
@@ -4555,10 +4561,10 @@
         <v>14</v>
       </c>
       <c r="C166" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D166" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
@@ -4569,10 +4575,10 @@
         <v>14</v>
       </c>
       <c r="C167" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="D167" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
@@ -4583,10 +4589,10 @@
         <v>14</v>
       </c>
       <c r="C168" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="D168" t="s">
-        <v>264</v>
+        <v>278</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
@@ -4597,10 +4603,10 @@
         <v>14</v>
       </c>
       <c r="C169" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="D169" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
@@ -4611,10 +4617,10 @@
         <v>14</v>
       </c>
       <c r="C170" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="D170" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
@@ -4625,10 +4631,10 @@
         <v>14</v>
       </c>
       <c r="C171" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D171" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
@@ -4639,10 +4645,10 @@
         <v>14</v>
       </c>
       <c r="C172" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D172" t="s">
-        <v>264</v>
+        <v>285</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
@@ -4653,10 +4659,10 @@
         <v>14</v>
       </c>
       <c r="C173" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="D173" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
@@ -4667,7 +4673,10 @@
         <v>14</v>
       </c>
       <c r="C174" t="s">
-        <v>293</v>
+        <v>288</v>
+      </c>
+      <c r="D174" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
@@ -4678,10 +4687,10 @@
         <v>14</v>
       </c>
       <c r="C175" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D175" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
@@ -4692,10 +4701,10 @@
         <v>14</v>
       </c>
       <c r="C176" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D176" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
@@ -4706,10 +4715,7 @@
         <v>14</v>
       </c>
       <c r="C177" t="s">
-        <v>297</v>
-      </c>
-      <c r="D177" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
@@ -4720,10 +4726,10 @@
         <v>14</v>
       </c>
       <c r="C178" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D178" t="s">
-        <v>300</v>
+        <v>263</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
@@ -4734,10 +4740,10 @@
         <v>14</v>
       </c>
       <c r="C179" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="D179" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
@@ -4748,10 +4754,10 @@
         <v>14</v>
       </c>
       <c r="C180" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="D180" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
@@ -4762,10 +4768,10 @@
         <v>14</v>
       </c>
       <c r="C181" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="D181" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
@@ -4776,10 +4782,10 @@
         <v>14</v>
       </c>
       <c r="C182" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="D182" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
@@ -4790,10 +4796,10 @@
         <v>14</v>
       </c>
       <c r="C183" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="D183" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
@@ -4804,10 +4810,10 @@
         <v>14</v>
       </c>
       <c r="C184" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="D184" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
@@ -4818,10 +4824,10 @@
         <v>14</v>
       </c>
       <c r="C185" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="D185" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
@@ -4832,10 +4838,10 @@
         <v>14</v>
       </c>
       <c r="C186" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="D186" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
@@ -4846,10 +4852,10 @@
         <v>14</v>
       </c>
       <c r="C187" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="D187" t="s">
-        <v>316</v>
+        <v>263</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
@@ -4860,10 +4866,10 @@
         <v>14</v>
       </c>
       <c r="C188" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="D188" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
@@ -4874,10 +4880,10 @@
         <v>14</v>
       </c>
       <c r="C189" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="D189" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
@@ -4888,10 +4894,10 @@
         <v>14</v>
       </c>
       <c r="C190" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="D190" t="s">
-        <v>298</v>
+        <v>315</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
@@ -4902,10 +4908,10 @@
         <v>14</v>
       </c>
       <c r="C191" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="D191" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
@@ -4916,10 +4922,10 @@
         <v>14</v>
       </c>
       <c r="C192" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="D192" t="s">
-        <v>52</v>
+        <v>319</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
@@ -4930,10 +4936,10 @@
         <v>14</v>
       </c>
       <c r="C193" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D193" t="s">
-        <v>326</v>
+        <v>297</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
@@ -4944,10 +4950,10 @@
         <v>14</v>
       </c>
       <c r="C194" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="D194" t="s">
-        <v>264</v>
+        <v>322</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
@@ -4958,10 +4964,10 @@
         <v>14</v>
       </c>
       <c r="C195" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D195" t="s">
-        <v>329</v>
+        <v>51</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
@@ -4972,7 +4978,10 @@
         <v>14</v>
       </c>
       <c r="C196" t="s">
-        <v>330</v>
+        <v>324</v>
+      </c>
+      <c r="D196" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
@@ -4983,10 +4992,10 @@
         <v>14</v>
       </c>
       <c r="C197" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="D197" t="s">
-        <v>298</v>
+        <v>263</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
@@ -4997,10 +5006,10 @@
         <v>14</v>
       </c>
       <c r="C198" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="D198" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
@@ -5011,10 +5020,7 @@
         <v>14</v>
       </c>
       <c r="C199" t="s">
-        <v>334</v>
-      </c>
-      <c r="D199" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
@@ -5025,10 +5031,10 @@
         <v>14</v>
       </c>
       <c r="C200" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="D200" t="s">
-        <v>264</v>
+        <v>297</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
@@ -5039,10 +5045,10 @@
         <v>14</v>
       </c>
       <c r="C201" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="D201" t="s">
-        <v>52</v>
+        <v>332</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
@@ -5053,10 +5059,10 @@
         <v>14</v>
       </c>
       <c r="C202" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D202" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
@@ -5067,10 +5073,10 @@
         <v>14</v>
       </c>
       <c r="C203" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D203" t="s">
-        <v>340</v>
+        <v>263</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
@@ -5081,10 +5087,10 @@
         <v>14</v>
       </c>
       <c r="C204" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="D204" t="s">
-        <v>342</v>
+        <v>51</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
@@ -5095,10 +5101,10 @@
         <v>14</v>
       </c>
       <c r="C205" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="D205" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
@@ -5109,10 +5115,10 @@
         <v>14</v>
       </c>
       <c r="C206" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="D206" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
@@ -5123,10 +5129,10 @@
         <v>14</v>
       </c>
       <c r="C207" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="D207" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
@@ -5137,10 +5143,10 @@
         <v>14</v>
       </c>
       <c r="C208" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="D208" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.2">
@@ -5151,10 +5157,10 @@
         <v>14</v>
       </c>
       <c r="C209" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D209" t="s">
-        <v>200</v>
+        <v>345</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
@@ -5165,10 +5171,10 @@
         <v>14</v>
       </c>
       <c r="C210" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="D210" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
@@ -5179,10 +5185,10 @@
         <v>14</v>
       </c>
       <c r="C211" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="D211" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
@@ -5193,10 +5199,10 @@
         <v>14</v>
       </c>
       <c r="C212" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="D212" t="s">
-        <v>264</v>
+        <v>199</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
@@ -5207,10 +5213,10 @@
         <v>14</v>
       </c>
       <c r="C213" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D213" t="s">
-        <v>264</v>
+        <v>351</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
@@ -5221,10 +5227,10 @@
         <v>14</v>
       </c>
       <c r="C214" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="D214" t="s">
-        <v>264</v>
+        <v>353</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.2">
@@ -5235,7 +5241,10 @@
         <v>14</v>
       </c>
       <c r="C215" t="s">
-        <v>358</v>
+        <v>354</v>
+      </c>
+      <c r="D215" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
@@ -5246,7 +5255,10 @@
         <v>14</v>
       </c>
       <c r="C216" t="s">
-        <v>359</v>
+        <v>355</v>
+      </c>
+      <c r="D216" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
@@ -5257,10 +5269,10 @@
         <v>14</v>
       </c>
       <c r="C217" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="D217" t="s">
-        <v>361</v>
+        <v>263</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
@@ -5271,10 +5283,7 @@
         <v>14</v>
       </c>
       <c r="C218" t="s">
-        <v>362</v>
-      </c>
-      <c r="D218" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
@@ -5285,10 +5294,7 @@
         <v>14</v>
       </c>
       <c r="C219" t="s">
-        <v>364</v>
-      </c>
-      <c r="D219" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
@@ -5299,10 +5305,10 @@
         <v>14</v>
       </c>
       <c r="C220" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="D220" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
@@ -5313,10 +5319,10 @@
         <v>14</v>
       </c>
       <c r="C221" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="D221" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
@@ -5327,7 +5333,10 @@
         <v>14</v>
       </c>
       <c r="C222" t="s">
-        <v>370</v>
+        <v>363</v>
+      </c>
+      <c r="D222" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
@@ -5338,7 +5347,10 @@
         <v>14</v>
       </c>
       <c r="C223" t="s">
-        <v>371</v>
+        <v>365</v>
+      </c>
+      <c r="D223" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
@@ -5349,10 +5361,10 @@
         <v>14</v>
       </c>
       <c r="C224" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="D224" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
@@ -5363,10 +5375,7 @@
         <v>14</v>
       </c>
       <c r="C225" t="s">
-        <v>374</v>
-      </c>
-      <c r="D225" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
@@ -5377,10 +5386,7 @@
         <v>14</v>
       </c>
       <c r="C226" t="s">
-        <v>376</v>
-      </c>
-      <c r="D226" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
@@ -5391,10 +5397,10 @@
         <v>14</v>
       </c>
       <c r="C227" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="D227" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
@@ -5405,10 +5411,10 @@
         <v>14</v>
       </c>
       <c r="C228" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="D228" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
@@ -5419,10 +5425,10 @@
         <v>14</v>
       </c>
       <c r="C229" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="D229" t="s">
-        <v>296</v>
+        <v>376</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
@@ -5433,7 +5439,10 @@
         <v>14</v>
       </c>
       <c r="C230" t="s">
-        <v>383</v>
+        <v>377</v>
+      </c>
+      <c r="D230" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
@@ -5444,10 +5453,10 @@
         <v>14</v>
       </c>
       <c r="C231" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="D231" t="s">
-        <v>42</v>
+        <v>380</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
@@ -5458,10 +5467,10 @@
         <v>14</v>
       </c>
       <c r="C232" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D232" t="s">
-        <v>386</v>
+        <v>295</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
@@ -5472,10 +5481,7 @@
         <v>14</v>
       </c>
       <c r="C233" t="s">
-        <v>387</v>
-      </c>
-      <c r="D233" t="s">
-        <v>269</v>
+        <v>382</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
@@ -5486,10 +5492,10 @@
         <v>14</v>
       </c>
       <c r="C234" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="D234" t="s">
-        <v>389</v>
+        <v>41</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
@@ -5500,10 +5506,10 @@
         <v>14</v>
       </c>
       <c r="C235" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="D235" t="s">
-        <v>48</v>
+        <v>385</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
@@ -5514,10 +5520,10 @@
         <v>14</v>
       </c>
       <c r="C236" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="D236" t="s">
-        <v>392</v>
+        <v>268</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
@@ -5528,10 +5534,10 @@
         <v>14</v>
       </c>
       <c r="C237" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="D237" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
@@ -5542,10 +5548,10 @@
         <v>14</v>
       </c>
       <c r="C238" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="D238" t="s">
-        <v>396</v>
+        <v>47</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
@@ -5556,10 +5562,10 @@
         <v>14</v>
       </c>
       <c r="C239" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="D239" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
@@ -5570,10 +5576,10 @@
         <v>14</v>
       </c>
       <c r="C240" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="D240" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
@@ -5584,10 +5590,10 @@
         <v>14</v>
       </c>
       <c r="C241" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="D241" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
@@ -5598,10 +5604,10 @@
         <v>14</v>
       </c>
       <c r="C242" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="D242" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
@@ -5612,10 +5618,10 @@
         <v>14</v>
       </c>
       <c r="C243" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="D243" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
@@ -5626,10 +5632,10 @@
         <v>14</v>
       </c>
       <c r="C244" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="D244" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
@@ -5640,10 +5646,10 @@
         <v>14</v>
       </c>
       <c r="C245" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="D245" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
@@ -5654,10 +5660,10 @@
         <v>14</v>
       </c>
       <c r="C246" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="D246" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
@@ -5668,7 +5674,10 @@
         <v>14</v>
       </c>
       <c r="C247" t="s">
-        <v>413</v>
+        <v>406</v>
+      </c>
+      <c r="D247" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
@@ -5679,10 +5688,10 @@
         <v>14</v>
       </c>
       <c r="C248" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="D248" t="s">
-        <v>132</v>
+        <v>409</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
@@ -5693,10 +5702,10 @@
         <v>14</v>
       </c>
       <c r="C249" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="D249" t="s">
-        <v>271</v>
+        <v>411</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
@@ -5707,10 +5716,7 @@
         <v>14</v>
       </c>
       <c r="C250" t="s">
-        <v>416</v>
-      </c>
-      <c r="D250" t="s">
-        <v>271</v>
+        <v>412</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
@@ -5721,10 +5727,10 @@
         <v>14</v>
       </c>
       <c r="C251" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D251" t="s">
-        <v>418</v>
+        <v>131</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.2">
@@ -5735,7 +5741,10 @@
         <v>14</v>
       </c>
       <c r="C252" t="s">
-        <v>419</v>
+        <v>414</v>
+      </c>
+      <c r="D252" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
@@ -5746,10 +5755,10 @@
         <v>14</v>
       </c>
       <c r="C253" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="D253" t="s">
-        <v>421</v>
+        <v>270</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
@@ -5760,10 +5769,10 @@
         <v>14</v>
       </c>
       <c r="C254" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="D254" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
@@ -5774,7 +5783,7 @@
         <v>14</v>
       </c>
       <c r="C255" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.2">
@@ -5785,7 +5794,10 @@
         <v>14</v>
       </c>
       <c r="C256" t="s">
-        <v>425</v>
+        <v>419</v>
+      </c>
+      <c r="D256" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.2">
@@ -5796,7 +5808,10 @@
         <v>14</v>
       </c>
       <c r="C257" t="s">
-        <v>426</v>
+        <v>421</v>
+      </c>
+      <c r="D257" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.2">
@@ -5807,10 +5822,7 @@
         <v>14</v>
       </c>
       <c r="C258" t="s">
-        <v>427</v>
-      </c>
-      <c r="D258" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.2">
@@ -5821,10 +5833,7 @@
         <v>14</v>
       </c>
       <c r="C259" t="s">
-        <v>429</v>
-      </c>
-      <c r="D259" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.2">
@@ -5835,10 +5844,7 @@
         <v>14</v>
       </c>
       <c r="C260" t="s">
-        <v>430</v>
-      </c>
-      <c r="D260" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.2">
@@ -5849,7 +5855,10 @@
         <v>14</v>
       </c>
       <c r="C261" t="s">
-        <v>431</v>
+        <v>426</v>
+      </c>
+      <c r="D261" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.2">
@@ -5860,7 +5869,10 @@
         <v>14</v>
       </c>
       <c r="C262" t="s">
-        <v>432</v>
+        <v>428</v>
+      </c>
+      <c r="D262" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.2">
@@ -5871,10 +5883,10 @@
         <v>14</v>
       </c>
       <c r="C263" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="D263" t="s">
-        <v>296</v>
+        <v>427</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.2">
@@ -5885,10 +5897,7 @@
         <v>14</v>
       </c>
       <c r="C264" t="s">
-        <v>434</v>
-      </c>
-      <c r="D264" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.2">
@@ -5899,10 +5908,7 @@
         <v>14</v>
       </c>
       <c r="C265" t="s">
-        <v>436</v>
-      </c>
-      <c r="D265" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.2">
@@ -5913,7 +5919,10 @@
         <v>14</v>
       </c>
       <c r="C266" t="s">
-        <v>438</v>
+        <v>432</v>
+      </c>
+      <c r="D266" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.2">
@@ -5924,10 +5933,10 @@
         <v>14</v>
       </c>
       <c r="C267" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="D267" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.2">
@@ -5938,10 +5947,10 @@
         <v>14</v>
       </c>
       <c r="C268" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="D268" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.2">
@@ -5952,10 +5961,7 @@
         <v>14</v>
       </c>
       <c r="C269" t="s">
-        <v>443</v>
-      </c>
-      <c r="D269" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.2">
@@ -5966,10 +5972,10 @@
         <v>14</v>
       </c>
       <c r="C270" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="D270" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.2">
@@ -5980,7 +5986,10 @@
         <v>14</v>
       </c>
       <c r="C271" t="s">
-        <v>447</v>
+        <v>440</v>
+      </c>
+      <c r="D271" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.2">
@@ -5991,10 +6000,10 @@
         <v>14</v>
       </c>
       <c r="C272" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="D272" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.2">
@@ -6005,10 +6014,10 @@
         <v>14</v>
       </c>
       <c r="C273" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="D273" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.2">
@@ -6019,10 +6028,7 @@
         <v>14</v>
       </c>
       <c r="C274" t="s">
-        <v>452</v>
-      </c>
-      <c r="D274" t="s">
-        <v>38</v>
+        <v>446</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.2">
@@ -6033,10 +6039,10 @@
         <v>14</v>
       </c>
       <c r="C275" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="D275" t="s">
-        <v>354</v>
+        <v>448</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.2">
@@ -6047,10 +6053,10 @@
         <v>14</v>
       </c>
       <c r="C276" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="D276" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.2">
@@ -6061,10 +6067,10 @@
         <v>14</v>
       </c>
       <c r="C277" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="D277" t="s">
-        <v>457</v>
+        <v>37</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.2">
@@ -6075,10 +6081,10 @@
         <v>14</v>
       </c>
       <c r="C278" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="D278" t="s">
-        <v>459</v>
+        <v>353</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.2">
@@ -6089,10 +6095,10 @@
         <v>14</v>
       </c>
       <c r="C279" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="D279" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.2">
@@ -6103,10 +6109,10 @@
         <v>14</v>
       </c>
       <c r="C280" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="D280" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.2">
@@ -6117,10 +6123,10 @@
         <v>14</v>
       </c>
       <c r="C281" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="D281" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.2">
@@ -6131,10 +6137,10 @@
         <v>14</v>
       </c>
       <c r="C282" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="D282" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.2">
@@ -6145,10 +6151,10 @@
         <v>14</v>
       </c>
       <c r="C283" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="D283" t="s">
-        <v>136</v>
+        <v>462</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.2">
@@ -6159,10 +6165,10 @@
         <v>14</v>
       </c>
       <c r="C284" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="D284" t="s">
-        <v>309</v>
+        <v>464</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.2">
@@ -6173,10 +6179,10 @@
         <v>14</v>
       </c>
       <c r="C285" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="D285" t="s">
-        <v>320</v>
+        <v>466</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.2">
@@ -6187,10 +6193,10 @@
         <v>14</v>
       </c>
       <c r="C286" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="D286" t="s">
-        <v>472</v>
+        <v>135</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.2">
@@ -6201,10 +6207,10 @@
         <v>14</v>
       </c>
       <c r="C287" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D287" t="s">
-        <v>62</v>
+        <v>308</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.2">
@@ -6215,10 +6221,10 @@
         <v>14</v>
       </c>
       <c r="C288" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="D288" t="s">
-        <v>126</v>
+        <v>319</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.2">
@@ -6229,7 +6235,10 @@
         <v>14</v>
       </c>
       <c r="C289" t="s">
-        <v>338</v>
+        <v>470</v>
+      </c>
+      <c r="D289" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.2">
@@ -6240,10 +6249,10 @@
         <v>14</v>
       </c>
       <c r="C290" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="D290" t="s">
-        <v>476</v>
+        <v>61</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.2">
@@ -6254,10 +6263,10 @@
         <v>14</v>
       </c>
       <c r="C291" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="D291" t="s">
-        <v>478</v>
+        <v>125</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.2">
@@ -6268,10 +6277,7 @@
         <v>14</v>
       </c>
       <c r="C292" t="s">
-        <v>479</v>
-      </c>
-      <c r="D292" t="s">
-        <v>132</v>
+        <v>337</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.2">
@@ -6282,10 +6288,10 @@
         <v>14</v>
       </c>
       <c r="C293" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="D293" t="s">
-        <v>455</v>
+        <v>475</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.2">
@@ -6296,10 +6302,10 @@
         <v>14</v>
       </c>
       <c r="C294" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="D294" t="s">
-        <v>459</v>
+        <v>477</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.2">
@@ -6310,10 +6316,10 @@
         <v>14</v>
       </c>
       <c r="C295" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="D295" t="s">
-        <v>461</v>
+        <v>131</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.2">
@@ -6324,10 +6330,10 @@
         <v>14</v>
       </c>
       <c r="C296" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="D296" t="s">
-        <v>62</v>
+        <v>454</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.2">
@@ -6338,10 +6344,10 @@
         <v>14</v>
       </c>
       <c r="C297" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="D297" t="s">
-        <v>126</v>
+        <v>458</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.2">
@@ -6352,10 +6358,10 @@
         <v>14</v>
       </c>
       <c r="C298" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="D298" t="s">
-        <v>486</v>
+        <v>460</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.2">
@@ -6366,10 +6372,10 @@
         <v>14</v>
       </c>
       <c r="C299" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="D299" t="s">
-        <v>132</v>
+        <v>61</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.2">
@@ -6380,10 +6386,10 @@
         <v>14</v>
       </c>
       <c r="C300" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="D300" t="s">
-        <v>488</v>
+        <v>125</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.2">
@@ -6394,10 +6400,10 @@
         <v>14</v>
       </c>
       <c r="C301" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="D301" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.2">
@@ -6408,10 +6414,10 @@
         <v>14</v>
       </c>
       <c r="C302" t="s">
-        <v>491</v>
+        <v>478</v>
       </c>
       <c r="D302" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.2">
@@ -6422,10 +6428,10 @@
         <v>14</v>
       </c>
       <c r="C303" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="D303" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.2">
@@ -6436,10 +6442,10 @@
         <v>14</v>
       </c>
       <c r="C304" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="D304" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.2">
@@ -6450,10 +6456,10 @@
         <v>14</v>
       </c>
       <c r="C305" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="D305" t="s">
-        <v>497</v>
+        <v>18</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.2">
@@ -6464,10 +6470,10 @@
         <v>14</v>
       </c>
       <c r="C306" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="D306" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.2">
@@ -6478,10 +6484,10 @@
         <v>14</v>
       </c>
       <c r="C307" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="D307" t="s">
-        <v>412</v>
+        <v>494</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.2">
@@ -6492,10 +6498,10 @@
         <v>14</v>
       </c>
       <c r="C308" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="D308" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.2">
@@ -6506,10 +6512,10 @@
         <v>14</v>
       </c>
       <c r="C309" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="D309" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.2">
@@ -6520,10 +6526,10 @@
         <v>14</v>
       </c>
       <c r="C310" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="D310" t="s">
-        <v>506</v>
+        <v>411</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.2">
@@ -6534,10 +6540,10 @@
         <v>14</v>
       </c>
       <c r="C311" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="D311" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.2">
@@ -6548,10 +6554,10 @@
         <v>14</v>
       </c>
       <c r="C312" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="D312" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.2">
@@ -6562,7 +6568,10 @@
         <v>14</v>
       </c>
       <c r="C313" t="s">
-        <v>511</v>
+        <v>504</v>
+      </c>
+      <c r="D313" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.2">
@@ -6573,7 +6582,10 @@
         <v>14</v>
       </c>
       <c r="C314" t="s">
-        <v>512</v>
+        <v>506</v>
+      </c>
+      <c r="D314" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.2">
@@ -6584,10 +6596,10 @@
         <v>14</v>
       </c>
       <c r="C315" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="D315" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.2">
@@ -6598,7 +6610,7 @@
         <v>14</v>
       </c>
       <c r="C316" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.2">
@@ -6609,10 +6621,7 @@
         <v>14</v>
       </c>
       <c r="C317" t="s">
-        <v>516</v>
-      </c>
-      <c r="D317" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.2">
@@ -6623,10 +6632,10 @@
         <v>14</v>
       </c>
       <c r="C318" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="D318" t="s">
-        <v>130</v>
+        <v>513</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.2">
@@ -6637,10 +6646,7 @@
         <v>14</v>
       </c>
       <c r="C319" t="s">
-        <v>519</v>
-      </c>
-      <c r="D319" t="s">
-        <v>52</v>
+        <v>514</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.2">
@@ -6651,7 +6657,10 @@
         <v>14</v>
       </c>
       <c r="C320" t="s">
-        <v>520</v>
+        <v>515</v>
+      </c>
+      <c r="D320" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.2">
@@ -6662,10 +6671,10 @@
         <v>14</v>
       </c>
       <c r="C321" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="D321" t="s">
-        <v>279</v>
+        <v>129</v>
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.2">
@@ -6676,7 +6685,10 @@
         <v>14</v>
       </c>
       <c r="C322" t="s">
-        <v>522</v>
+        <v>518</v>
+      </c>
+      <c r="D322" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.2">
@@ -6687,7 +6699,7 @@
         <v>14</v>
       </c>
       <c r="C323" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.2">
@@ -6698,10 +6710,10 @@
         <v>14</v>
       </c>
       <c r="C324" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="D324" t="s">
-        <v>298</v>
+        <v>278</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.2">
@@ -6712,10 +6724,7 @@
         <v>14</v>
       </c>
       <c r="C325" t="s">
-        <v>525</v>
-      </c>
-      <c r="D325" t="s">
-        <v>298</v>
+        <v>521</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.2">
@@ -6726,10 +6735,7 @@
         <v>14</v>
       </c>
       <c r="C326" t="s">
-        <v>526</v>
-      </c>
-      <c r="D326" t="s">
-        <v>298</v>
+        <v>522</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.2">
@@ -6740,10 +6746,10 @@
         <v>14</v>
       </c>
       <c r="C327" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="D327" t="s">
-        <v>528</v>
+        <v>297</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.2">
@@ -6754,7 +6760,10 @@
         <v>14</v>
       </c>
       <c r="C328" t="s">
-        <v>529</v>
+        <v>524</v>
+      </c>
+      <c r="D328" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.2">
@@ -6765,10 +6774,10 @@
         <v>14</v>
       </c>
       <c r="C329" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="D329" t="s">
-        <v>320</v>
+        <v>297</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.2">
@@ -6779,10 +6788,10 @@
         <v>14</v>
       </c>
       <c r="C330" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="D330" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.2">
@@ -6793,10 +6802,7 @@
         <v>14</v>
       </c>
       <c r="C331" t="s">
-        <v>533</v>
-      </c>
-      <c r="D331" t="s">
-        <v>264</v>
+        <v>528</v>
       </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.2">
@@ -6807,10 +6813,10 @@
         <v>14</v>
       </c>
       <c r="C332" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="D332" t="s">
-        <v>277</v>
+        <v>319</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.2">
@@ -6821,10 +6827,10 @@
         <v>14</v>
       </c>
       <c r="C333" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="D333" t="s">
-        <v>264</v>
+        <v>531</v>
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.2">
@@ -6835,10 +6841,10 @@
         <v>14</v>
       </c>
       <c r="C334" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="D334" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.2">
@@ -6849,10 +6855,10 @@
         <v>14</v>
       </c>
       <c r="C335" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="D335" t="s">
-        <v>264</v>
+        <v>276</v>
       </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.2">
@@ -6863,10 +6869,10 @@
         <v>14</v>
       </c>
       <c r="C336" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="D336" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.2">
@@ -6877,10 +6883,10 @@
         <v>14</v>
       </c>
       <c r="C337" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="D337" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.2">
@@ -6891,7 +6897,10 @@
         <v>14</v>
       </c>
       <c r="C338" t="s">
-        <v>540</v>
+        <v>536</v>
+      </c>
+      <c r="D338" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.2">
@@ -6902,10 +6911,10 @@
         <v>14</v>
       </c>
       <c r="C339" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="D339" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.2">
@@ -6916,10 +6925,10 @@
         <v>14</v>
       </c>
       <c r="C340" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="D340" t="s">
-        <v>543</v>
+        <v>263</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.2">
@@ -6930,10 +6939,7 @@
         <v>14</v>
       </c>
       <c r="C341" t="s">
-        <v>544</v>
-      </c>
-      <c r="D341" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.2">
@@ -6944,10 +6950,10 @@
         <v>14</v>
       </c>
       <c r="C342" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="D342" t="s">
-        <v>404</v>
+        <v>263</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.2">
@@ -6958,10 +6964,10 @@
         <v>14</v>
       </c>
       <c r="C343" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="D343" t="s">
-        <v>404</v>
+        <v>542</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.2">
@@ -6972,10 +6978,10 @@
         <v>14</v>
       </c>
       <c r="C344" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="D344" t="s">
-        <v>300</v>
+        <v>544</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.2">
@@ -6986,10 +6992,10 @@
         <v>14</v>
       </c>
       <c r="C345" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="D345" t="s">
-        <v>550</v>
+        <v>403</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.2">
@@ -7000,10 +7006,10 @@
         <v>14</v>
       </c>
       <c r="C346" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="D346" t="s">
-        <v>122</v>
+        <v>403</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.2">
@@ -7014,10 +7020,10 @@
         <v>14</v>
       </c>
       <c r="C347" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="D347" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.2">
@@ -7028,10 +7034,10 @@
         <v>14</v>
       </c>
       <c r="C348" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="D348" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.2">
@@ -7042,10 +7048,10 @@
         <v>14</v>
       </c>
       <c r="C349" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="D349" t="s">
-        <v>556</v>
+        <v>121</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.2">
@@ -7056,10 +7062,10 @@
         <v>14</v>
       </c>
       <c r="C350" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="D350" t="s">
-        <v>558</v>
+        <v>263</v>
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.2">
@@ -7070,10 +7076,10 @@
         <v>14</v>
       </c>
       <c r="C351" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="D351" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.2">
@@ -7084,10 +7090,10 @@
         <v>14</v>
       </c>
       <c r="C352" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="D352" t="s">
-        <v>562</v>
+        <v>555</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.2">
@@ -7098,10 +7104,10 @@
         <v>14</v>
       </c>
       <c r="C353" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="D353" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.2">
@@ -7112,10 +7118,10 @@
         <v>14</v>
       </c>
       <c r="C354" t="s">
-        <v>565</v>
+        <v>558</v>
       </c>
       <c r="D354" t="s">
-        <v>292</v>
+        <v>559</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.2">
@@ -7126,10 +7132,10 @@
         <v>14</v>
       </c>
       <c r="C355" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="D355" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.2">
@@ -7140,10 +7146,10 @@
         <v>14</v>
       </c>
       <c r="C356" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="D356" t="s">
-        <v>517</v>
+        <v>563</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.2">
@@ -7154,10 +7160,10 @@
         <v>14</v>
       </c>
       <c r="C357" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="D357" t="s">
-        <v>570</v>
+        <v>291</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.2">
@@ -7168,10 +7174,10 @@
         <v>14</v>
       </c>
       <c r="C358" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="D358" t="s">
-        <v>264</v>
+        <v>566</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.2">
@@ -7182,7 +7188,10 @@
         <v>14</v>
       </c>
       <c r="C359" t="s">
-        <v>572</v>
+        <v>567</v>
+      </c>
+      <c r="D359" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.2">
@@ -7193,10 +7202,10 @@
         <v>14</v>
       </c>
       <c r="C360" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="D360" t="s">
-        <v>298</v>
+        <v>569</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.2">
@@ -7207,10 +7216,10 @@
         <v>14</v>
       </c>
       <c r="C361" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="D361" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.2">
@@ -7221,10 +7230,7 @@
         <v>14</v>
       </c>
       <c r="C362" t="s">
-        <v>575</v>
-      </c>
-      <c r="D362" t="s">
-        <v>264</v>
+        <v>571</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.2">
@@ -7235,7 +7241,10 @@
         <v>14</v>
       </c>
       <c r="C363" t="s">
-        <v>576</v>
+        <v>572</v>
+      </c>
+      <c r="D363" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.2">
@@ -7246,7 +7255,10 @@
         <v>14</v>
       </c>
       <c r="C364" t="s">
-        <v>577</v>
+        <v>573</v>
+      </c>
+      <c r="D364" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.2">
@@ -7257,7 +7269,10 @@
         <v>14</v>
       </c>
       <c r="C365" t="s">
-        <v>578</v>
+        <v>574</v>
+      </c>
+      <c r="D365" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.2">
@@ -7268,10 +7283,7 @@
         <v>14</v>
       </c>
       <c r="C366" t="s">
-        <v>579</v>
-      </c>
-      <c r="D366" t="s">
-        <v>264</v>
+        <v>575</v>
       </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.2">
@@ -7282,7 +7294,7 @@
         <v>14</v>
       </c>
       <c r="C367" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.2">
@@ -7293,10 +7305,7 @@
         <v>14</v>
       </c>
       <c r="C368" t="s">
-        <v>581</v>
-      </c>
-      <c r="D368" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.2">
@@ -7307,10 +7316,10 @@
         <v>14</v>
       </c>
       <c r="C369" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="D369" t="s">
-        <v>584</v>
+        <v>263</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.2">
@@ -7321,10 +7330,7 @@
         <v>14</v>
       </c>
       <c r="C370" t="s">
-        <v>585</v>
-      </c>
-      <c r="D370" t="s">
-        <v>586</v>
+        <v>579</v>
       </c>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.2">
@@ -7335,7 +7341,10 @@
         <v>14</v>
       </c>
       <c r="C371" t="s">
-        <v>587</v>
+        <v>580</v>
+      </c>
+      <c r="D371" t="s">
+        <v>581</v>
       </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.2">
@@ -7346,10 +7355,10 @@
         <v>14</v>
       </c>
       <c r="C372" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="D372" t="s">
-        <v>404</v>
+        <v>583</v>
       </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.2">
@@ -7360,10 +7369,10 @@
         <v>14</v>
       </c>
       <c r="C373" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="D373" t="s">
-        <v>302</v>
+        <v>585</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.2">
@@ -7374,10 +7383,7 @@
         <v>14</v>
       </c>
       <c r="C374" t="s">
-        <v>590</v>
-      </c>
-      <c r="D374" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.2">
@@ -7388,10 +7394,10 @@
         <v>14</v>
       </c>
       <c r="C375" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="D375" t="s">
-        <v>264</v>
+        <v>403</v>
       </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.2">
@@ -7402,7 +7408,10 @@
         <v>14</v>
       </c>
       <c r="C376" t="s">
-        <v>593</v>
+        <v>588</v>
+      </c>
+      <c r="D376" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.2">
@@ -7413,10 +7422,10 @@
         <v>14</v>
       </c>
       <c r="C377" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="D377" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.2">
@@ -7427,10 +7436,10 @@
         <v>14</v>
       </c>
       <c r="C378" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="D378" t="s">
-        <v>428</v>
+        <v>263</v>
       </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.2">
@@ -7441,10 +7450,7 @@
         <v>14</v>
       </c>
       <c r="C379" t="s">
-        <v>597</v>
-      </c>
-      <c r="D379" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.2">
@@ -7455,10 +7461,10 @@
         <v>14</v>
       </c>
       <c r="C380" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="D380" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.2">
@@ -7469,10 +7475,10 @@
         <v>14</v>
       </c>
       <c r="C381" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="D381" t="s">
-        <v>600</v>
+        <v>427</v>
       </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.2">
@@ -7483,10 +7489,10 @@
         <v>14</v>
       </c>
       <c r="C382" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="D382" t="s">
-        <v>602</v>
+        <v>594</v>
       </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.2">
@@ -7497,10 +7503,10 @@
         <v>14</v>
       </c>
       <c r="C383" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="D383" t="s">
-        <v>52</v>
+        <v>594</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.2">
@@ -7511,10 +7517,10 @@
         <v>14</v>
       </c>
       <c r="C384" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="D384" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.2">
@@ -7525,10 +7531,10 @@
         <v>14</v>
       </c>
       <c r="C385" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="D385" t="s">
-        <v>595</v>
+        <v>601</v>
       </c>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.2">
@@ -7539,10 +7545,10 @@
         <v>14</v>
       </c>
       <c r="C386" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="D386" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.2">
@@ -7553,10 +7559,52 @@
         <v>14</v>
       </c>
       <c r="C387" t="s">
+        <v>603</v>
+      </c>
+      <c r="D387" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="388" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A388" t="s">
+        <v>13</v>
+      </c>
+      <c r="B388" t="s">
+        <v>14</v>
+      </c>
+      <c r="C388" t="s">
+        <v>605</v>
+      </c>
+      <c r="D388" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="389" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A389" t="s">
+        <v>13</v>
+      </c>
+      <c r="B389" t="s">
+        <v>14</v>
+      </c>
+      <c r="C389" t="s">
+        <v>606</v>
+      </c>
+      <c r="D389" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="390" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A390" t="s">
+        <v>13</v>
+      </c>
+      <c r="B390" t="s">
+        <v>14</v>
+      </c>
+      <c r="C390" t="s">
+        <v>607</v>
+      </c>
+      <c r="D390" t="s">
         <v>608</v>
-      </c>
-      <c r="D387" t="s">
-        <v>609</v>
       </c>
     </row>
   </sheetData>

</xml_diff>